<commit_message>
Made Excel Table more realistic
</commit_message>
<xml_diff>
--- a/WPF-GUI-Localizer/Example_Excel/Resource/Language_File.xlsx
+++ b/WPF-GUI-Localizer/Example_Excel/Resource/Language_File.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4644"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="17256" windowHeight="4644"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Dialog</t>
   </si>
@@ -59,30 +59,12 @@
     <t>Add new</t>
   </si>
   <si>
-    <t>sv--Add new</t>
-  </si>
-  <si>
-    <t>de--Add new</t>
-  </si>
-  <si>
-    <t>fr--Add new</t>
-  </si>
-  <si>
     <t>WoTButton</t>
   </si>
   <si>
     <t>Click here for Wall of Text</t>
   </si>
   <si>
-    <t>sv--Click here for Wall of Text</t>
-  </si>
-  <si>
-    <t>de--Click here for Wall of Text</t>
-  </si>
-  <si>
-    <t>fr--Click here for Wall of Text</t>
-  </si>
-  <si>
     <t>TextBlock</t>
   </si>
   <si>
@@ -92,15 +74,6 @@
     <t>Please read the following Wall of Text</t>
   </si>
   <si>
-    <t>sv--Please read the following Wall of Text</t>
-  </si>
-  <si>
-    <t>de--Please read the following Wall of Text</t>
-  </si>
-  <si>
-    <t>fr--Please read the following Wall of Text</t>
-  </si>
-  <si>
     <t>CheckBox</t>
   </si>
   <si>
@@ -110,57 +83,21 @@
     <t>Yes I have read the Wall of Text</t>
   </si>
   <si>
-    <t>sv--Yes I have read the Wall of Text</t>
-  </si>
-  <si>
-    <t>de--Yes I have read the Wall of Text</t>
-  </si>
-  <si>
-    <t>fr--Yes I have read the Wall of Text</t>
-  </si>
-  <si>
     <t>Save</t>
   </si>
   <si>
     <t>Save List</t>
   </si>
   <si>
-    <t>sv--Save List</t>
-  </si>
-  <si>
-    <t>de--Save List</t>
-  </si>
-  <si>
-    <t>fr--Save List</t>
-  </si>
-  <si>
     <t>Remove</t>
   </si>
   <si>
     <t>Remove selected</t>
   </si>
   <si>
-    <t>sv--Remove selected</t>
-  </si>
-  <si>
-    <t>de--Remove selected</t>
-  </si>
-  <si>
-    <t>fr--Remove selected</t>
-  </si>
-  <si>
     <t>Edit</t>
   </si>
   <si>
-    <t>sv--Edit</t>
-  </si>
-  <si>
-    <t>de--Edit</t>
-  </si>
-  <si>
-    <t>fr--Edit</t>
-  </si>
-  <si>
     <t>DataGridColumn</t>
   </si>
   <si>
@@ -170,75 +107,30 @@
     <t>Supplier Website</t>
   </si>
   <si>
-    <t>sv--Supplier Website</t>
-  </si>
-  <si>
-    <t>de--Supplier Website</t>
-  </si>
-  <si>
-    <t>fr--Supplier Website</t>
-  </si>
-  <si>
     <t>dgcReceived</t>
   </si>
   <si>
     <t>Received</t>
   </si>
   <si>
-    <t>sv--Received</t>
-  </si>
-  <si>
-    <t>de--Received</t>
-  </si>
-  <si>
-    <t>fr--Received</t>
-  </si>
-  <si>
     <t>dgcName</t>
   </si>
   <si>
     <t>Item Name</t>
   </si>
   <si>
-    <t>sv--Item Name</t>
-  </si>
-  <si>
-    <t>de--Item Name</t>
-  </si>
-  <si>
-    <t>fr--Item Name</t>
-  </si>
-  <si>
     <t>dgcQuantity</t>
   </si>
   <si>
     <t>Item Quantity</t>
   </si>
   <si>
-    <t>sv--Item Quantity</t>
-  </si>
-  <si>
-    <t>de--Item Quantity</t>
-  </si>
-  <si>
-    <t>fr--Item Quantity</t>
-  </si>
-  <si>
     <t>TableSelectionLabel</t>
   </si>
   <si>
     <t>Please choose a table to view\nthe following tables are lists of orders\npreviously created</t>
   </si>
   <si>
-    <t>sv--Please choose a table to view\nthe following tables are lists of orders\npreviously created</t>
-  </si>
-  <si>
-    <t>de--Please choose a table to view\nthe following tables are lists of orders\npreviously created</t>
-  </si>
-  <si>
-    <t>fr--Please choose a table to view\nthe following tables are lists of orders\npreviously created</t>
-  </si>
-  <si>
     <t>Newest</t>
   </si>
   <si>
@@ -254,16 +146,16 @@
     <t>Neuestes</t>
   </si>
   <si>
-    <t>Nèwést</t>
-  </si>
-  <si>
-    <t>Samé Table again</t>
-  </si>
-  <si>
-    <t>Säme Table ägain</t>
-  </si>
-  <si>
-    <t>hej</t>
+    <t>Nyaste</t>
+  </si>
+  <si>
+    <t>Le plus récent</t>
+  </si>
+  <si>
+    <t>Même table à nouveau</t>
+  </si>
+  <si>
+    <t>Samma tabell igen</t>
   </si>
 </sst>
 </file>
@@ -636,15 +528,6 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -654,19 +537,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -674,22 +548,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -697,22 +562,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -723,19 +579,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -746,19 +593,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -769,19 +607,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -789,22 +618,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -812,22 +632,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -835,22 +646,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -858,22 +660,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -881,56 +674,47 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small corrections to Example Projects
</commit_message>
<xml_diff>
--- a/WPF-GUI-Localizer/Example_Excel/Resource/Language_File.xlsx
+++ b/WPF-GUI-Localizer/Example_Excel/Resource/Language_File.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="17256" windowHeight="4644"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="17256" windowHeight="4644"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>gloss</t>
   </si>
   <si>
-    <t>Selbe Tabelle nocheinmal</t>
-  </si>
-  <si>
     <t>Neuestes</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>Samma tabell igen</t>
+  </si>
+  <si>
+    <t>Selbe Tabelle noch einmal</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,13 +691,13 @@
         <v>35</v>
       </c>
       <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
         <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -708,13 +708,13 @@
         <v>36</v>
       </c>
       <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
         <v>43</v>
       </c>
-      <c r="F15" t="s">
-        <v>38</v>
-      </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>